<commit_message>
Worked on temporal resolution
</commit_message>
<xml_diff>
--- a/Input/urbs_intertemporal_2050/2029.xlsx
+++ b/Input/urbs_intertemporal_2050/2029.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\Desktop\urbsextension\Input\urbs_intertemporal_2050\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\GitHub\urbs-extension\Input\urbs_intertemporal_2050\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73CE0C3-B236-4DDF-998B-D3A9D6DC7FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65E32DA-1A77-4A0B-93B9-79CE97ACE314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29760" yWindow="960" windowWidth="28800" windowHeight="15285" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -857,9 +857,9 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -881,7 +881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -901,13 +901,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>87</v>
       </c>
@@ -921,7 +921,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -935,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -949,7 +949,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -963,7 +963,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -977,7 +977,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -991,7 +991,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -1119,9 +1119,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
@@ -1143,9 +1143,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
@@ -1167,9 +1167,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1198,9 +1198,9 @@
       <selection activeCell="D6" sqref="D6:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1397,9 +1397,9 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>9</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>9</v>
       </c>
@@ -1923,9 +1923,9 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>0.246</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>0.47851999999999989</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>96</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>96</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>96</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>97</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>97</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>97</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>98</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>98</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>98</v>
       </c>
@@ -2461,9 +2461,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -2521,9 +2521,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>3.4999999999999999E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2773,9 +2773,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -2805,15 +2805,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
@@ -2821,7 +2824,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2829,12 +2832,100 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3423812500</v>
+        <v>285317708</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>285317708</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>285317708</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>285317708</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>285317708</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>285317708</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>285317708</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>285317708</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>285317708</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>285317708</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>285317708</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>285317708</v>
       </c>
     </row>
   </sheetData>

</xml_diff>